<commit_message>
Refactor plotting and add uncertainty calculation script
Refactored main.py to focus on a single plot, improved error bar handling, and added theoretical curve visualization. Introduced unc.py for detailed resistance uncertainty calculations. Minor update in voltage.py to print S1 for debugging. Updated related figures and data files.
</commit_message>
<xml_diff>
--- a/Exp-elecbridge/data/工作簿1.xlsx
+++ b/Exp-elecbridge/data/工作簿1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Study\大二上\exp\Exp-elecbridge\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D00FA87-29A4-49F7-8FAE-6BBBDF1AC183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F99326A1-0716-441C-933B-BAF312C64043}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{C8803BF8-2B12-47F8-A076-6F615D32ECD7}"/>
+    <workbookView xWindow="368" yWindow="368" windowWidth="17999" windowHeight="10432" xr2:uid="{C8803BF8-2B12-47F8-A076-6F615D32ECD7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
     <t>E(V)</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -53,11 +53,31 @@
     <t>R0'(欧)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>S</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R2(欧)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R1/R2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rx(欧)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <numFmts count="2">
+    <numFmt numFmtId="177" formatCode="0.0_ "/>
+    <numFmt numFmtId="178" formatCode="0.0_);[Red]\(0.0\)"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -83,7 +103,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -91,18 +111,57 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -440,127 +499,257 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E96AC3A2-EA4B-443F-9FED-9E009262A170}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="6.86328125" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="7.796875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="7.46484375" customWidth="1"/>
+    <col min="5" max="5" width="3.9296875" customWidth="1"/>
+    <col min="6" max="6" width="5.796875" customWidth="1"/>
+    <col min="7" max="7" width="8.1328125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="7.9296875" style="4" customWidth="1"/>
+    <col min="9" max="9" width="6.86328125" customWidth="1"/>
+    <col min="10" max="10" width="4" customWidth="1"/>
+    <col min="11" max="11" width="5.19921875" customWidth="1"/>
+    <col min="12" max="12" width="8.1328125" style="5" customWidth="1"/>
+    <col min="13" max="13" width="8.1328125" style="4" customWidth="1"/>
+    <col min="14" max="14" width="6.33203125" customWidth="1"/>
+    <col min="15" max="15" width="9.06640625" style="4"/>
+    <col min="16" max="16" width="7.53125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="I1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A2" s="3">
         <v>900</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="7">
         <v>61469</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="7">
         <v>61669</v>
       </c>
-      <c r="E2">
+      <c r="D2" s="3">
+        <v>122.938</v>
+      </c>
+      <c r="F2" s="3">
         <v>2.5</v>
       </c>
-      <c r="F2">
+      <c r="G2" s="7">
         <v>61583</v>
       </c>
-      <c r="G2">
+      <c r="H2" s="7">
         <v>61883</v>
       </c>
+      <c r="I2" s="3">
+        <v>82.110667000000007</v>
+      </c>
+      <c r="K2" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="L2" s="9">
+        <v>900</v>
+      </c>
+      <c r="M2" s="7">
+        <v>9000</v>
+      </c>
+      <c r="N2" s="3">
+        <f>L2/M2</f>
+        <v>0.1</v>
+      </c>
+      <c r="O2" s="7">
+        <v>61199</v>
+      </c>
+      <c r="P2" s="3">
+        <f>O2/M2*L2</f>
+        <v>6119.9</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A3" s="3">
         <v>1000</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="7">
         <v>61719</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="7">
         <v>61919</v>
       </c>
-      <c r="E3">
+      <c r="D3" s="3">
+        <v>123.438</v>
+      </c>
+      <c r="F3" s="3">
         <v>2</v>
       </c>
-      <c r="F3">
+      <c r="G3" s="7">
         <v>61383</v>
       </c>
-      <c r="G3">
+      <c r="H3" s="7">
         <v>61983</v>
       </c>
+      <c r="I3" s="3">
+        <v>40.921999999999997</v>
+      </c>
+      <c r="K3" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="L3" s="9">
+        <v>10000</v>
+      </c>
+      <c r="M3" s="7">
+        <v>30000</v>
+      </c>
+      <c r="N3" s="3">
+        <f t="shared" ref="N3:N4" si="0">L3/M3</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="O3" s="7">
+        <v>625.4</v>
+      </c>
+      <c r="P3" s="3">
+        <f t="shared" ref="P3:P4" si="1">O3/M3*L3</f>
+        <v>208.46666666666667</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A4">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A4" s="3">
         <v>2000</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="7">
         <v>61509</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="7">
         <v>61809</v>
       </c>
-      <c r="E4">
+      <c r="D4" s="3">
+        <v>82.012</v>
+      </c>
+      <c r="F4" s="3">
         <v>1.5</v>
       </c>
-      <c r="F4">
+      <c r="G4" s="7">
         <v>61483</v>
       </c>
-      <c r="G4">
+      <c r="H4" s="7">
         <v>61933</v>
       </c>
+      <c r="I4" s="3">
+        <v>54.651555999999999</v>
+      </c>
+      <c r="K4" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="L4" s="9">
+        <v>90</v>
+      </c>
+      <c r="M4" s="7">
+        <v>20000</v>
+      </c>
+      <c r="N4" s="3">
+        <f t="shared" si="0"/>
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="O4" s="7">
+        <v>3274</v>
+      </c>
+      <c r="P4" s="3">
+        <f t="shared" si="1"/>
+        <v>14.733000000000001</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A5">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A5" s="3">
         <v>3000</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="7">
         <v>61609</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="7">
         <v>61905</v>
       </c>
-      <c r="E5">
+      <c r="D5" s="3">
+        <v>83.255405409999995</v>
+      </c>
+      <c r="F5" s="3">
         <v>1</v>
       </c>
-      <c r="F5">
+      <c r="G5" s="7">
         <v>61199</v>
       </c>
-      <c r="G5">
+      <c r="H5" s="7">
         <v>62199</v>
       </c>
+      <c r="I5" s="3">
+        <v>24.479600000000001</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A6">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A6" s="3">
         <v>5000</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="7">
         <v>61543</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="7">
         <v>61883</v>
+      </c>
+      <c r="D6" s="3">
+        <v>72.403529410000004</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>